<commit_message>
upload pdf visualization testing result
</commit_message>
<xml_diff>
--- a/app/pdf/test/pdf_table.xlsx
+++ b/app/pdf/test/pdf_table.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="subset" sheetId="1" r:id="rId1"/>
-    <sheet name="total" sheetId="2" r:id="rId2"/>
+    <sheet name="total-1" sheetId="2" r:id="rId2"/>
+    <sheet name="total-2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="190">
   <si>
     <t>Tube voltage</t>
   </si>
@@ -266,16 +267,226 @@
     <t>NXG150</t>
   </si>
   <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>1.90</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>2.53</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>2.81</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>1.46</t>
+  </si>
+  <si>
+    <t>3.39</t>
+  </si>
+  <si>
+    <t>3.95</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>1.64</t>
+  </si>
+  <si>
+    <t>3.62</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>1.84</t>
+  </si>
+  <si>
+    <t>4.04</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>2.05</t>
+  </si>
+  <si>
+    <t>5.49</t>
+  </si>
+  <si>
+    <t>6.61</t>
+  </si>
+  <si>
+    <t>5.56</t>
+  </si>
+  <si>
+    <t>7.59</t>
+  </si>
+  <si>
+    <t>10.31</t>
+  </si>
+  <si>
+    <t>6.33</t>
+  </si>
+  <si>
+    <t>7.20</t>
+  </si>
+  <si>
+    <t>7.58</t>
+  </si>
+  <si>
+    <t>8.83</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>NXD200</t>
+  </si>
+  <si>
+    <t>NXE200</t>
+  </si>
+  <si>
     <t>NXG200</t>
   </si>
   <si>
     <t>NXH200</t>
   </si>
   <si>
-    <t>NXD200</t>
-  </si>
-  <si>
-    <t>NXE200</t>
+    <t>NXE250</t>
   </si>
   <si>
     <t>NXF250</t>
@@ -287,9 +498,6 @@
     <t>NXI250</t>
   </si>
   <si>
-    <t>NXE250</t>
-  </si>
-  <si>
     <t>NXF280</t>
   </si>
   <si>
@@ -320,151 +528,13 @@
     <t>5.0</t>
   </si>
   <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
-    <t>1.90</t>
-  </si>
-  <si>
-    <t>0.68</t>
-  </si>
-  <si>
-    <t>1.12</t>
-  </si>
-  <si>
-    <t>2.53</t>
-  </si>
-  <si>
-    <t>0.79</t>
-  </si>
-  <si>
-    <t>1.29</t>
-  </si>
-  <si>
-    <t>2.81</t>
-  </si>
-  <si>
-    <t>0.90</t>
-  </si>
-  <si>
-    <t>1.46</t>
-  </si>
-  <si>
-    <t>3.39</t>
-  </si>
-  <si>
-    <t>3.95</t>
-  </si>
-  <si>
-    <t>1.02</t>
-  </si>
-  <si>
-    <t>1.64</t>
-  </si>
-  <si>
-    <t>3.62</t>
-  </si>
-  <si>
-    <t>1.15</t>
-  </si>
-  <si>
-    <t>1.84</t>
-  </si>
-  <si>
-    <t>4.04</t>
-  </si>
-  <si>
-    <t>1.30</t>
-  </si>
-  <si>
-    <t>2.05</t>
-  </si>
-  <si>
-    <t>5.49</t>
-  </si>
-  <si>
-    <t>6.61</t>
-  </si>
-  <si>
-    <t>5.56</t>
-  </si>
-  <si>
-    <t>7.59</t>
-  </si>
-  <si>
-    <t>10.31</t>
-  </si>
-  <si>
-    <t>6.33</t>
-  </si>
-  <si>
-    <t>7.20</t>
-  </si>
-  <si>
-    <t>7.58</t>
-  </si>
-  <si>
-    <t>8.83</t>
-  </si>
-  <si>
     <t>10.53</t>
   </si>
   <si>
-    <t>0.06</t>
-  </si>
-  <si>
-    <t>0.10</t>
-  </si>
-  <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>0.14</t>
-  </si>
-  <si>
-    <t>0.13</t>
-  </si>
-  <si>
-    <t>0.15</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>0.23</t>
-  </si>
-  <si>
-    <t>0.37</t>
-  </si>
-  <si>
-    <t>0.63</t>
-  </si>
-  <si>
-    <t>0.34</t>
-  </si>
-  <si>
-    <t>0.77</t>
-  </si>
-  <si>
-    <t>1.03</t>
-  </si>
-  <si>
-    <t>0.38</t>
-  </si>
-  <si>
-    <t>0.49</t>
-  </si>
-  <si>
-    <t>1.13</t>
-  </si>
-  <si>
-    <t>1.38</t>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>1.21</t>
   </si>
   <si>
     <t>2.00</t>
@@ -473,10 +543,7 @@
     <t>2.54</t>
   </si>
   <si>
-    <t>0.73</t>
-  </si>
-  <si>
-    <t>1.21</t>
+    <t>1.61</t>
   </si>
   <si>
     <t>2.14</t>
@@ -488,9 +555,6 @@
     <t>3.60</t>
   </si>
   <si>
-    <t>1.61</t>
-  </si>
-  <si>
     <t>2.43</t>
   </si>
   <si>
@@ -510,69 +574,6 @@
   </si>
   <si>
     <t>4.34</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>2.7</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>2.6</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>4.8</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>4.3</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>2.8</t>
-  </si>
-  <si>
-    <t>0.9</t>
   </si>
   <si>
     <t>2.9</t>
@@ -1320,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1370,7 +1371,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
@@ -1398,14 +1399,14 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
         <v>20.93</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="I3" s="2">
         <v>48.72</v>
@@ -1426,16 +1427,16 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="G4" s="2">
         <v>27.07</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="I4" s="2">
         <v>46.7</v>
@@ -1456,14 +1457,14 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
         <v>19.5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="I5" s="2">
         <v>50.2</v>
@@ -1484,7 +1485,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
@@ -1542,7 +1543,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>34</v>
@@ -1551,7 +1552,7 @@
         <v>30.62</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="I8" s="2">
         <v>46.46</v>
@@ -1572,14 +1573,14 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
         <v>20.86</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="I9" s="2">
         <v>49.69</v>
@@ -1600,14 +1601,14 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
         <v>24.09</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="I10" s="2">
         <v>47.98</v>
@@ -1628,16 +1629,16 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="G11" s="2">
         <v>32.25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="I11" s="2">
         <v>46.59</v>
@@ -1658,14 +1659,14 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
         <v>22.15</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="I12" s="2">
         <v>49.3</v>
@@ -1686,14 +1687,14 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
         <v>25.44</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="I13" s="2">
         <v>47.79</v>
@@ -1744,16 +1745,16 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="G15" s="2">
         <v>35.19</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="I15" s="2">
         <v>46.61</v>
@@ -1774,10 +1775,10 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="G16" s="2">
         <v>37.51</v>
@@ -1804,14 +1805,14 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
         <v>23.48</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="I17" s="2">
         <v>48.99</v>
@@ -1832,14 +1833,14 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
         <v>26.84</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="I18" s="2">
         <v>47.65</v>
@@ -1860,16 +1861,16 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="G19" s="2">
         <v>36.33</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="I19" s="2">
         <v>46.71</v>
@@ -1890,14 +1891,14 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
         <v>24.88</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="I20" s="2">
         <v>48.72</v>
@@ -1918,14 +1919,14 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
         <v>28.32</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="I21" s="2">
         <v>47.54</v>
@@ -1946,10 +1947,10 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="G22" s="2">
         <v>38.38</v>
@@ -1976,14 +1977,14 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
         <v>26.34</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="I23" s="2">
         <v>48.53</v>
@@ -2004,14 +2005,14 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
         <v>29.87</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="I24" s="2">
         <v>47.46</v>
@@ -2062,16 +2063,16 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="G26" s="2">
         <v>44.58</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="I26" s="2">
         <v>46.92</v>
@@ -2092,10 +2093,10 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="G27" s="2">
         <v>49.08</v>
@@ -2122,16 +2123,16 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="G28" s="2">
         <v>45.74</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="I28" s="2">
         <v>46.94</v>
@@ -2182,16 +2183,16 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="G30" s="2">
         <v>53.75</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="I30" s="2">
         <v>47.14</v>
@@ -2214,16 +2215,16 @@
         <v>25</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="G31" s="2">
         <v>65</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="I31" s="2">
         <v>47.46</v>
@@ -2244,7 +2245,7 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>37</v>
@@ -2274,16 +2275,16 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="G33" s="2">
         <v>53.14</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="I33" s="2">
         <v>47.07</v>
@@ -2337,13 +2338,13 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="G35" s="2">
         <v>69.84999999999999</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="I35" s="2">
         <v>47.5</v>
@@ -2367,13 +2368,13 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="G36" s="2">
         <v>78.52</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="I36" s="2">
         <v>47.6</v>
@@ -2394,16 +2395,16 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="G37" s="2">
         <v>55.19</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="I37" s="2">
         <v>47.11</v>
@@ -2424,16 +2425,16 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="G38" s="2">
         <v>60.13</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="I38" s="2">
         <v>47.24</v>
@@ -2487,13 +2488,13 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="G40" s="2">
         <v>81.36</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="I40" s="2">
         <v>47.61</v>
@@ -2517,7 +2518,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="G41" s="2">
         <v>89.06999999999999</v>
@@ -2532,663 +2533,708 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="2">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="2">
         <v>200</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="2">
+        <v>69.76000000000001</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="2">
+        <v>47.34</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="2">
+        <v>200</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="2">
+        <v>82.81</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="2">
+        <v>47.57</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2">
+        <v>200</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="2">
+        <v>94.73999999999999</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G42" s="2">
+      <c r="I4" s="2">
+        <v>47.64</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="2">
+        <v>200</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="2">
         <v>105.25</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="2">
+        <v>200</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="2">
+        <v>120.15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I6" s="2">
+        <v>47.69</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="2">
+        <v>250</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="2">
+        <v>92.84</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2">
+        <v>47.58</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="2">
+        <v>250</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="2">
+        <v>107.32</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I8" s="2">
+        <v>47.68</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2">
+        <v>250</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="2">
+        <v>120.1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="2">
+        <v>250</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="2">
+        <v>137.46</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" s="2">
+        <v>47.78</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="2">
+        <v>250</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="2">
+        <v>149.51</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" s="2">
+        <v>47.75</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="2">
+        <v>280</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="2">
+        <v>114.61</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I12" s="2">
+        <v>47.66</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="2">
+        <v>280</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="2">
+        <v>128.5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I13" s="2">
+        <v>47.7</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2">
+        <v>280</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="2">
+        <v>147.05</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="2">
+        <v>47.76</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="2">
+        <v>280</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I42" s="2">
-        <v>47.7</v>
-      </c>
-      <c r="J42" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="2">
-        <v>200</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="G15" s="2">
+        <v>159.92</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I15" s="2">
+        <v>47.72</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="2">
+        <v>300</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="2">
+        <v>133.92</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I16" s="2">
+        <v>47.66</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2">
+        <v>300</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G43" s="2">
-        <v>120.15</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="I43" s="2">
-        <v>47.69</v>
-      </c>
-      <c r="J43" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="2">
-        <v>200</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="2">
+        <v>153.21</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="2">
+        <v>47.65</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="2">
+        <v>300</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G18" s="2">
+        <v>166.58</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G44" s="2">
-        <v>69.76000000000001</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I44" s="2">
-        <v>47.34</v>
-      </c>
-      <c r="J44" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="2">
-        <v>200</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G45" s="2">
-        <v>82.81</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I45" s="2">
-        <v>47.57</v>
-      </c>
-      <c r="J45" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="2">
-        <v>200</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G46" s="2">
-        <v>94.73999999999999</v>
-      </c>
-      <c r="H46" s="2" t="s">
+      <c r="I18" s="2">
+        <v>47.64</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="2">
+        <v>320</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G19" s="2">
+        <v>159.22</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I46" s="2">
-        <v>47.64</v>
-      </c>
-      <c r="J46" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="2">
+      <c r="I19" s="2">
+        <v>47.58</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="2">
+        <v>320</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="2">
+        <v>173.06</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I20" s="2">
+        <v>47.56</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="2">
         <v>250</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G47" s="2">
-        <v>107.32</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I47" s="2">
-        <v>47.68</v>
-      </c>
-      <c r="J47" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="2">
-        <v>250</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G21" s="2">
         <v>120.1</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I48" s="2">
-        <v>47.7</v>
-      </c>
-      <c r="J48" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="2">
-        <v>250</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="I21" s="2">
+        <v>47.6</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="2">
+        <v>280</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G49" s="2">
-        <v>137.46</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="I49" s="2">
-        <v>47.78</v>
-      </c>
-      <c r="J49" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="2">
-        <v>250</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" s="2">
-        <v>149.51</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="I50" s="2">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="2">
+        <v>147.05</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="2">
+        <v>47.79</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2">
+        <v>300</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="2">
+        <v>153.21</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="2">
         <v>47.75</v>
       </c>
-      <c r="J50" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="2">
-        <v>250</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G51" s="2">
-        <v>92.84</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I51" s="2">
-        <v>47.58</v>
-      </c>
-      <c r="J51" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="2">
-        <v>280</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G52" s="2">
-        <v>114.61</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I52" s="2">
-        <v>47.66</v>
-      </c>
-      <c r="J52" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="2">
-        <v>280</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G53" s="2">
-        <v>128.5</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I53" s="2">
-        <v>47.7</v>
-      </c>
-      <c r="J53" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" s="2">
-        <v>280</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G54" s="2">
-        <v>147.05</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I54" s="2">
-        <v>47.76</v>
-      </c>
-      <c r="J54" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="2">
-        <v>280</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G55" s="2">
-        <v>159.92</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I55" s="2">
-        <v>47.72</v>
-      </c>
-      <c r="J55" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="2">
-        <v>300</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G56" s="2">
-        <v>133.92</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I56" s="2">
-        <v>47.66</v>
-      </c>
-      <c r="J56" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="2">
-        <v>300</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G57" s="2">
-        <v>153.21</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I57" s="2">
-        <v>47.65</v>
-      </c>
-      <c r="J57" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B58" s="2">
-        <v>300</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G58" s="2">
-        <v>166.58</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I58" s="2">
-        <v>47.64</v>
-      </c>
-      <c r="J58" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" s="2">
-        <v>320</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G59" s="2">
-        <v>159.22</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I59" s="2">
-        <v>47.58</v>
-      </c>
-      <c r="J59" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="2">
-        <v>320</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G60" s="2">
-        <v>173.06</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I60" s="2">
-        <v>47.56</v>
-      </c>
-      <c r="J60" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="2">
-        <v>250</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G61" s="2">
-        <v>120.1</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I61" s="2">
-        <v>47.6</v>
-      </c>
-      <c r="J61" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B62" s="2">
-        <v>280</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G62" s="2">
-        <v>147.05</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I62" s="2">
-        <v>47.79</v>
-      </c>
-      <c r="J62" s="2">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B63" s="2">
-        <v>300</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G63" s="2">
-        <v>153.21</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I63" s="2">
-        <v>47.75</v>
-      </c>
-      <c r="J63" s="2">
+      <c r="J23" s="2">
         <v>1.4</v>
       </c>
     </row>

</xml_diff>